<commit_message>
Requirements and classification update
</commit_message>
<xml_diff>
--- a/xlslist/Acc_Xgboost.xlsx
+++ b/xlslist/Acc_Xgboost.xlsx
@@ -1,17 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>N. Classes</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NC_gen+NC_pr</t>
+  </si>
+  <si>
+    <t>SL+GC+NC(genome)</t>
+  </si>
+  <si>
+    <t>SL+GC+NC(proteome)</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Phylum</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50,89 +93,22 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -425,7 +401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +409,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -449,148 +425,191 @@
       <c r="F1" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Classification</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>N. Classes</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Samples</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NC</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>SQ+GC+NC</t>
-        </is>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Phylum</t>
-        </is>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>215</v>
+        <v>660</v>
       </c>
       <c r="E3" t="n">
-        <v>74.41860465116279</v>
+        <v>64.24242424242424</v>
       </c>
       <c r="F3" t="n">
-        <v>77.90697674418605</v>
+        <v>76.81818181818181</v>
+      </c>
+      <c r="G3" t="n">
+        <v>96.81818181818181</v>
+      </c>
+      <c r="H3" t="n">
+        <v>78.03030303030303</v>
+      </c>
+      <c r="I3" t="n">
+        <v>96.06060606060606</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Class</t>
-        </is>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>168</v>
+        <v>493</v>
       </c>
       <c r="E4" t="n">
-        <v>69.11764705882352</v>
+        <v>55.35353535353536</v>
       </c>
       <c r="F4" t="n">
-        <v>70.58823529411765</v>
+        <v>73.13131313131314</v>
+      </c>
+      <c r="G4" t="n">
+        <v>94.34343434343434</v>
+      </c>
+      <c r="H4" t="n">
+        <v>69.89898989898991</v>
+      </c>
+      <c r="I4" t="n">
+        <v>94.94949494949495</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Order</t>
-        </is>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" t="n">
-        <v>242</v>
+        <v>743</v>
       </c>
       <c r="E5" t="n">
-        <v>30.92783505154639</v>
+        <v>35.43624161073826</v>
       </c>
       <c r="F5" t="n">
-        <v>43.29896907216495</v>
+        <v>43.22147651006712</v>
+      </c>
+      <c r="G5" t="n">
+        <v>68.45637583892618</v>
+      </c>
+      <c r="H5" t="n">
+        <v>37.58389261744966</v>
+      </c>
+      <c r="I5" t="n">
+        <v>66.84563758389262</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Family</t>
-        </is>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>219</v>
+        <v>636</v>
       </c>
       <c r="E6" t="n">
-        <v>38.63636363636363</v>
+        <v>39.6875</v>
       </c>
       <c r="F6" t="n">
-        <v>43.18181818181818</v>
+        <v>55.46875</v>
+      </c>
+      <c r="G6" t="n">
+        <v>85.9375</v>
+      </c>
+      <c r="H6" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="I6" t="n">
+        <v>85.9375</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Genus</t>
-        </is>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="D7" t="n">
-        <v>213</v>
+        <v>543</v>
       </c>
       <c r="E7" t="n">
-        <v>23.25581395348837</v>
+        <v>40</v>
       </c>
       <c r="F7" t="n">
-        <v>24.41860465116279</v>
+        <v>54.86238532110092</v>
+      </c>
+      <c r="G7" t="n">
+        <v>93.02752293577981</v>
+      </c>
+      <c r="H7" t="n">
+        <v>47.15596330275229</v>
+      </c>
+      <c r="I7" t="n">
+        <v>93.21100917431193</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new features, and evaluation
</commit_message>
<xml_diff>
--- a/xlslist/Acc_Xgboost.xlsx
+++ b/xlslist/Acc_Xgboost.xlsx
@@ -401,7 +401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,7 +409,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -434,8 +434,11 @@
       <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -464,7 +467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -478,22 +481,25 @@
         <v>660</v>
       </c>
       <c r="E3" t="n">
-        <v>64.24242424242424</v>
+        <v>65.75757575757578</v>
       </c>
       <c r="F3" t="n">
-        <v>76.81818181818181</v>
+        <v>76.45454545454548</v>
       </c>
       <c r="G3" t="n">
-        <v>96.81818181818181</v>
+        <v>75.62121212121212</v>
       </c>
       <c r="H3" t="n">
-        <v>78.03030303030303</v>
+        <v>95.63636363636358</v>
       </c>
       <c r="I3" t="n">
-        <v>96.06060606060606</v>
+        <v>96.09090909090905</v>
+      </c>
+      <c r="J3" t="n">
+        <v>95.95454545454541</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -507,22 +513,25 @@
         <v>493</v>
       </c>
       <c r="E4" t="n">
-        <v>55.35353535353536</v>
+        <v>57.4949494949495</v>
       </c>
       <c r="F4" t="n">
-        <v>73.13131313131314</v>
+        <v>71.53535353535351</v>
       </c>
       <c r="G4" t="n">
-        <v>94.34343434343434</v>
+        <v>71.17171717171715</v>
       </c>
       <c r="H4" t="n">
-        <v>69.89898989898991</v>
+        <v>94.7474747474747</v>
       </c>
       <c r="I4" t="n">
-        <v>94.94949494949495</v>
+        <v>94.92929292929288</v>
+      </c>
+      <c r="J4" t="n">
+        <v>95.07070707070702</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -536,22 +545,25 @@
         <v>743</v>
       </c>
       <c r="E5" t="n">
-        <v>35.43624161073826</v>
+        <v>35.30201342281879</v>
       </c>
       <c r="F5" t="n">
-        <v>43.22147651006712</v>
+        <v>43.04697986577183</v>
       </c>
       <c r="G5" t="n">
-        <v>68.45637583892618</v>
+        <v>37.48993288590604</v>
       </c>
       <c r="H5" t="n">
-        <v>37.58389261744966</v>
+        <v>68.60402684563758</v>
       </c>
       <c r="I5" t="n">
-        <v>66.84563758389262</v>
+        <v>68.63087248322147</v>
+      </c>
+      <c r="J5" t="n">
+        <v>66.93959731543625</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -565,22 +577,25 @@
         <v>636</v>
       </c>
       <c r="E6" t="n">
-        <v>39.6875</v>
+        <v>39.40625</v>
       </c>
       <c r="F6" t="n">
-        <v>55.46875</v>
+        <v>54.04687500000001</v>
       </c>
       <c r="G6" t="n">
-        <v>85.9375</v>
+        <v>47.4375</v>
       </c>
       <c r="H6" t="n">
-        <v>48.75</v>
+        <v>85.796875</v>
       </c>
       <c r="I6" t="n">
         <v>85.9375</v>
       </c>
+      <c r="J6" t="n">
+        <v>85.703125</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -594,19 +609,22 @@
         <v>543</v>
       </c>
       <c r="E7" t="n">
-        <v>40</v>
+        <v>37.46788990825689</v>
       </c>
       <c r="F7" t="n">
-        <v>54.86238532110092</v>
+        <v>52.49541284403671</v>
       </c>
       <c r="G7" t="n">
-        <v>93.02752293577981</v>
+        <v>47.8348623853211</v>
       </c>
       <c r="H7" t="n">
-        <v>47.15596330275229</v>
+        <v>91.81651376146789</v>
       </c>
       <c r="I7" t="n">
-        <v>93.21100917431193</v>
+        <v>91.50458715596329</v>
+      </c>
+      <c r="J7" t="n">
+        <v>91.57798165137613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>